<commit_message>
making biplots highlighting samples in/outside interval
the samples outside the interval are scattered across the graphs --> no clear indication that one element is constantly over- or underestimated
</commit_message>
<xml_diff>
--- a/_BIPLOTS/area5.xlsx
+++ b/_BIPLOTS/area5.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF180"/>
+  <dimension ref="A1:AG180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,11 @@
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
+          <t>interval</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
           <t>area</t>
         </is>
       </c>
@@ -637,7 +642,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG2" t="n">
         <v>5</v>
       </c>
     </row>
@@ -755,7 +765,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF3" t="n">
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG3" t="n">
         <v>5</v>
       </c>
     </row>
@@ -877,7 +892,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF4" t="n">
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -995,7 +1015,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF5" t="n">
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1113,7 +1138,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF6" t="n">
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG6" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1227,7 +1257,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF7" t="n">
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG7" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1345,7 +1380,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF8" t="n">
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1467,7 +1507,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF9" t="n">
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG9" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1589,7 +1634,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF10" t="n">
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG10" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1707,7 +1757,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF11" t="n">
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG11" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1821,7 +1876,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF12" t="n">
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG12" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1931,7 +1991,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF13" t="n">
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG13" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2049,7 +2114,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF14" t="n">
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG14" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2163,7 +2233,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF15" t="n">
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG15" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2281,7 +2356,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF16" t="n">
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG16" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2395,7 +2475,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF17" t="n">
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG17" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2513,7 +2598,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF18" t="n">
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG18" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2623,7 +2713,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF19" t="n">
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AG19" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2741,7 +2836,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF20" t="n">
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG20" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2855,7 +2955,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF21" t="n">
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG21" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2965,7 +3070,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF22" t="n">
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG22" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3075,7 +3185,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF23" t="n">
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG23" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3193,7 +3308,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF24" t="n">
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG24" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3311,7 +3431,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF25" t="n">
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG25" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3425,7 +3550,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF26" t="n">
+      <c r="AF26" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG26" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3543,7 +3673,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF27" t="n">
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG27" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3661,7 +3796,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF28" t="n">
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG28" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3775,7 +3915,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF29" t="n">
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG29" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3885,7 +4030,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF30" t="n">
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AG30" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4003,7 +4153,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF31" t="n">
+      <c r="AF31" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG31" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4121,7 +4276,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF32" t="n">
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG32" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4235,7 +4395,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF33" t="n">
+      <c r="AF33" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG33" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4353,7 +4518,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF34" t="n">
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG34" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4467,7 +4637,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF35" t="n">
+      <c r="AF35" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG35" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4589,7 +4764,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF36" t="n">
+      <c r="AF36" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG36" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4703,7 +4883,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF37" t="n">
+      <c r="AF37" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG37" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4821,7 +5006,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF38" t="n">
+      <c r="AF38" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG38" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4943,7 +5133,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF39" t="n">
+      <c r="AF39" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG39" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5065,7 +5260,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF40" t="n">
+      <c r="AF40" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG40" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5183,7 +5383,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF41" t="n">
+      <c r="AF41" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5305,7 +5510,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF42" t="n">
+      <c r="AF42" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG42" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5423,7 +5633,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF43" t="n">
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG43" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5545,7 +5760,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF44" t="n">
+      <c r="AF44" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG44" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5667,7 +5887,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF45" t="n">
+      <c r="AF45" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG45" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5781,7 +6006,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF46" t="n">
+      <c r="AF46" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG46" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5903,7 +6133,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF47" t="n">
+      <c r="AF47" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG47" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6021,7 +6256,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF48" t="n">
+      <c r="AF48" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG48" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6139,7 +6379,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF49" t="n">
+      <c r="AF49" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG49" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6253,7 +6498,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF50" t="n">
+      <c r="AF50" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG50" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6371,7 +6621,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF51" t="n">
+      <c r="AF51" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG51" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6485,7 +6740,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF52" t="n">
+      <c r="AF52" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG52" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6603,7 +6863,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF53" t="n">
+      <c r="AF53" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG53" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6725,7 +6990,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF54" t="n">
+      <c r="AF54" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG54" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6843,7 +7113,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF55" t="n">
+      <c r="AF55" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG55" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6957,7 +7232,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF56" t="n">
+      <c r="AF56" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG56" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7071,7 +7351,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF57" t="n">
+      <c r="AF57" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG57" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7185,7 +7470,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF58" t="n">
+      <c r="AF58" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG58" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7303,7 +7593,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF59" t="n">
+      <c r="AF59" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG59" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7417,7 +7712,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF60" t="n">
+      <c r="AF60" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AG60" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7531,7 +7831,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF61" t="n">
+      <c r="AF61" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG61" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7649,7 +7954,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF62" t="n">
+      <c r="AF62" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG62" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7767,7 +8077,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF63" t="n">
+      <c r="AF63" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG63" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7889,7 +8204,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF64" t="n">
+      <c r="AF64" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG64" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8007,7 +8327,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF65" t="n">
+      <c r="AF65" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG65" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8125,7 +8450,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF66" t="n">
+      <c r="AF66" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AG66" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8243,7 +8573,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF67" t="n">
+      <c r="AF67" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG67" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8361,7 +8696,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF68" t="n">
+      <c r="AF68" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG68" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8479,7 +8819,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF69" t="n">
+      <c r="AF69" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG69" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8593,7 +8938,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF70" t="n">
+      <c r="AF70" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG70" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8707,7 +9057,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF71" t="n">
+      <c r="AF71" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG71" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8825,7 +9180,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF72" t="n">
+      <c r="AF72" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG72" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8943,7 +9303,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF73" t="n">
+      <c r="AF73" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG73" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9057,7 +9422,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF74" t="n">
+      <c r="AF74" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG74" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9179,7 +9549,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF75" t="n">
+      <c r="AF75" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG75" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9297,7 +9672,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF76" t="n">
+      <c r="AF76" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG76" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9415,7 +9795,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF77" t="n">
+      <c r="AF77" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG77" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9533,7 +9918,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF78" t="n">
+      <c r="AF78" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG78" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9651,7 +10041,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF79" t="n">
+      <c r="AF79" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG79" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9765,7 +10160,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF80" t="n">
+      <c r="AF80" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG80" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9883,7 +10283,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF81" t="n">
+      <c r="AF81" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG81" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10001,7 +10406,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF82" t="n">
+      <c r="AF82" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG82" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10115,7 +10525,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF83" t="n">
+      <c r="AF83" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG83" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10229,7 +10644,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF84" t="n">
+      <c r="AF84" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG84" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10343,7 +10763,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF85" t="n">
+      <c r="AF85" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG85" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10461,7 +10886,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF86" t="n">
+      <c r="AF86" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG86" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10579,7 +11009,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF87" t="n">
+      <c r="AF87" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG87" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10693,7 +11128,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF88" t="n">
+      <c r="AF88" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG88" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10807,7 +11247,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF89" t="n">
+      <c r="AF89" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG89" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10925,7 +11370,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF90" t="n">
+      <c r="AF90" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG90" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11047,7 +11497,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF91" t="n">
+      <c r="AF91" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG91" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11165,7 +11620,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF92" t="n">
+      <c r="AF92" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG92" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11279,7 +11739,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF93" t="n">
+      <c r="AF93" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG93" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11393,7 +11858,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF94" t="n">
+      <c r="AF94" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG94" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11507,7 +11977,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF95" t="n">
+      <c r="AF95" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG95" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11621,7 +12096,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF96" t="n">
+      <c r="AF96" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG96" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11743,7 +12223,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF97" t="n">
+      <c r="AF97" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG97" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11861,7 +12346,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF98" t="n">
+      <c r="AF98" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG98" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11979,7 +12469,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF99" t="n">
+      <c r="AF99" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG99" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12093,7 +12588,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF100" t="n">
+      <c r="AF100" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG100" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12211,7 +12711,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF101" t="n">
+      <c r="AF101" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG101" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12329,7 +12834,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF102" t="n">
+      <c r="AF102" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG102" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12451,7 +12961,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF103" t="n">
+      <c r="AF103" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG103" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12569,7 +13084,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF104" t="n">
+      <c r="AF104" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG104" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12687,7 +13207,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF105" t="n">
+      <c r="AF105" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG105" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12805,7 +13330,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF106" t="n">
+      <c r="AF106" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG106" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12923,7 +13453,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF107" t="n">
+      <c r="AF107" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG107" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13041,7 +13576,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF108" t="n">
+      <c r="AF108" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG108" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13159,7 +13699,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF109" t="n">
+      <c r="AF109" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG109" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13281,7 +13826,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF110" t="n">
+      <c r="AF110" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG110" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13395,7 +13945,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF111" t="n">
+      <c r="AF111" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG111" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13509,7 +14064,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF112" t="n">
+      <c r="AF112" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG112" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13631,7 +14191,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF113" t="n">
+      <c r="AF113" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG113" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13753,7 +14318,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF114" t="n">
+      <c r="AF114" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG114" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13863,7 +14433,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF115" t="n">
+      <c r="AF115" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG115" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13977,7 +14552,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF116" t="n">
+      <c r="AF116" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG116" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14099,7 +14679,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF117" t="n">
+      <c r="AF117" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG117" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14213,7 +14798,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF118" t="n">
+      <c r="AF118" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG118" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14323,7 +14913,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF119" t="n">
+      <c r="AF119" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG119" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14437,7 +15032,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF120" t="n">
+      <c r="AF120" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG120" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14555,7 +15155,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF121" t="n">
+      <c r="AF121" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG121" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14677,7 +15282,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF122" t="n">
+      <c r="AF122" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG122" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14799,7 +15409,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF123" t="n">
+      <c r="AF123" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG123" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14909,7 +15524,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF124" t="n">
+      <c r="AF124" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG124" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15023,7 +15643,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF125" t="n">
+      <c r="AF125" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG125" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15141,7 +15766,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF126" t="n">
+      <c r="AF126" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG126" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15263,7 +15893,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF127" t="n">
+      <c r="AF127" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG127" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15377,7 +16012,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF128" t="n">
+      <c r="AF128" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG128" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15495,7 +16135,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF129" t="n">
+      <c r="AF129" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG129" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15613,7 +16258,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF130" t="n">
+      <c r="AF130" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG130" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15731,7 +16381,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF131" t="n">
+      <c r="AF131" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG131" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15849,7 +16504,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF132" t="n">
+      <c r="AF132" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG132" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15963,7 +16623,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF133" t="n">
+      <c r="AF133" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG133" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16085,7 +16750,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF134" t="n">
+      <c r="AF134" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG134" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16203,7 +16873,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF135" t="n">
+      <c r="AF135" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG135" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16321,7 +16996,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF136" t="n">
+      <c r="AF136" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG136" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16439,7 +17119,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF137" t="n">
+      <c r="AF137" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG137" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16553,7 +17238,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF138" t="n">
+      <c r="AF138" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG138" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16671,7 +17361,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF139" t="n">
+      <c r="AF139" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG139" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16785,7 +17480,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF140" t="n">
+      <c r="AF140" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG140" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16907,7 +17607,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF141" t="n">
+      <c r="AF141" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG141" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17021,7 +17726,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF142" t="n">
+      <c r="AF142" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG142" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17143,7 +17853,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF143" t="n">
+      <c r="AF143" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG143" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17261,7 +17976,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF144" t="n">
+      <c r="AF144" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG144" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17375,7 +18095,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF145" t="n">
+      <c r="AF145" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG145" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17497,7 +18222,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF146" t="n">
+      <c r="AF146" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG146" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17611,7 +18341,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF147" t="n">
+      <c r="AF147" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG147" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17729,7 +18464,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF148" t="n">
+      <c r="AF148" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG148" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17843,7 +18583,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF149" t="n">
+      <c r="AF149" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG149" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17957,7 +18702,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF150" t="n">
+      <c r="AF150" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG150" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18075,7 +18825,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF151" t="n">
+      <c r="AF151" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG151" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18185,7 +18940,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF152" t="n">
+      <c r="AF152" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG152" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18303,7 +19063,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF153" t="n">
+      <c r="AF153" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG153" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18417,7 +19182,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF154" t="n">
+      <c r="AF154" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG154" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18535,7 +19305,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF155" t="n">
+      <c r="AF155" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG155" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18649,7 +19424,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF156" t="n">
+      <c r="AF156" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG156" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18763,7 +19543,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF157" t="n">
+      <c r="AF157" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG157" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18881,7 +19666,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF158" t="n">
+      <c r="AF158" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG158" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18999,7 +19789,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF159" t="n">
+      <c r="AF159" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG159" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19117,7 +19912,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF160" t="n">
+      <c r="AF160" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AG160" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19235,7 +20035,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF161" t="n">
+      <c r="AF161" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG161" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19353,7 +20158,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF162" t="n">
+      <c r="AF162" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG162" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19467,7 +20277,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF163" t="n">
+      <c r="AF163" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG163" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19581,7 +20396,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF164" t="n">
+      <c r="AF164" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AG164" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19699,7 +20519,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF165" t="n">
+      <c r="AF165" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG165" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19813,7 +20638,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF166" t="n">
+      <c r="AF166" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG166" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19931,7 +20761,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF167" t="n">
+      <c r="AF167" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG167" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20041,7 +20876,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF168" t="n">
+      <c r="AF168" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG168" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20159,7 +20999,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF169" t="n">
+      <c r="AF169" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AG169" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20273,7 +21118,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF170" t="n">
+      <c r="AF170" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG170" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20387,7 +21237,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF171" t="n">
+      <c r="AF171" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG171" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20505,7 +21360,12 @@
           <t>mineral</t>
         </is>
       </c>
-      <c r="AF172" t="n">
+      <c r="AF172" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG172" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20623,7 +21483,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF173" t="n">
+      <c r="AF173" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG173" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20741,7 +21606,12 @@
           <t>no_zero</t>
         </is>
       </c>
-      <c r="AF174" t="n">
+      <c r="AF174" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG174" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20855,7 +21725,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF175" t="n">
+      <c r="AF175" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG175" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20965,7 +21840,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF176" t="n">
+      <c r="AF176" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG176" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21079,7 +21959,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF177" t="n">
+      <c r="AF177" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG177" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21197,7 +22082,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF178" t="n">
+      <c r="AF178" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG178" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21315,7 +22205,12 @@
           <t>oth</t>
         </is>
       </c>
-      <c r="AF179" t="n">
+      <c r="AF179" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG179" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21429,7 +22324,12 @@
           <t>mineraloth</t>
         </is>
       </c>
-      <c r="AF180" t="n">
+      <c r="AF180" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AG180" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
biplots highlighting samples in/outside finer interval
points outside the interval 99.75-100.5 were highlighted, same conclusion as interval 99.5-100.75
</commit_message>
<xml_diff>
--- a/_BIPLOTS/area5.xlsx
+++ b/_BIPLOTS/area5.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG180"/>
+  <dimension ref="A1:AH180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,11 @@
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
+          <t>interval_fine</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
           <t>area</t>
         </is>
       </c>
@@ -647,7 +652,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH2" t="n">
         <v>5</v>
       </c>
     </row>
@@ -770,7 +780,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG3" t="n">
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH3" t="n">
         <v>5</v>
       </c>
     </row>
@@ -897,7 +912,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG4" t="n">
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1020,7 +1040,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG5" t="n">
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1143,7 +1168,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG6" t="n">
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH6" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1262,7 +1292,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG7" t="n">
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH7" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1385,7 +1420,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG8" t="n">
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1512,7 +1552,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG9" t="n">
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH9" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1639,7 +1684,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG10" t="n">
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH10" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1762,7 +1812,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG11" t="n">
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH11" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1881,7 +1936,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG12" t="n">
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH12" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1996,7 +2056,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG13" t="n">
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH13" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2119,7 +2184,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG14" t="n">
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH14" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2238,7 +2308,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG15" t="n">
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH15" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2361,7 +2436,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG16" t="n">
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH16" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2480,7 +2560,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG17" t="n">
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH17" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2603,7 +2688,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG18" t="n">
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH18" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2718,7 +2808,12 @@
           <t>outside</t>
         </is>
       </c>
-      <c r="AG19" t="n">
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH19" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2841,7 +2936,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG20" t="n">
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH20" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2960,7 +3060,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG21" t="n">
+      <c r="AG21" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH21" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3075,7 +3180,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG22" t="n">
+      <c r="AG22" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH22" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3190,7 +3300,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG23" t="n">
+      <c r="AG23" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH23" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3313,7 +3428,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG24" t="n">
+      <c r="AG24" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH24" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3436,7 +3556,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG25" t="n">
+      <c r="AG25" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH25" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3555,7 +3680,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG26" t="n">
+      <c r="AG26" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH26" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3678,7 +3808,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG27" t="n">
+      <c r="AG27" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH27" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3801,7 +3936,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG28" t="n">
+      <c r="AG28" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH28" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3920,7 +4060,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG29" t="n">
+      <c r="AG29" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH29" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4035,7 +4180,12 @@
           <t>outside</t>
         </is>
       </c>
-      <c r="AG30" t="n">
+      <c r="AG30" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH30" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4158,7 +4308,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG31" t="n">
+      <c r="AG31" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH31" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4281,7 +4436,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG32" t="n">
+      <c r="AG32" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH32" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4400,7 +4560,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG33" t="n">
+      <c r="AG33" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH33" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4523,7 +4688,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG34" t="n">
+      <c r="AG34" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH34" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4642,7 +4812,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG35" t="n">
+      <c r="AG35" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH35" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4769,7 +4944,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG36" t="n">
+      <c r="AG36" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH36" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4888,7 +5068,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG37" t="n">
+      <c r="AG37" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH37" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5011,7 +5196,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG38" t="n">
+      <c r="AG38" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH38" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5138,7 +5328,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG39" t="n">
+      <c r="AG39" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH39" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5265,7 +5460,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG40" t="n">
+      <c r="AG40" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH40" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5388,7 +5588,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG41" t="n">
+      <c r="AG41" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5515,7 +5720,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG42" t="n">
+      <c r="AG42" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH42" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5638,7 +5848,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG43" t="n">
+      <c r="AG43" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH43" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5765,7 +5980,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG44" t="n">
+      <c r="AG44" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH44" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5892,7 +6112,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG45" t="n">
+      <c r="AG45" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH45" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6011,7 +6236,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG46" t="n">
+      <c r="AG46" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH46" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6138,7 +6368,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG47" t="n">
+      <c r="AG47" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH47" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6261,7 +6496,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG48" t="n">
+      <c r="AG48" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH48" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6384,7 +6624,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG49" t="n">
+      <c r="AG49" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH49" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6503,7 +6748,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG50" t="n">
+      <c r="AG50" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH50" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6626,7 +6876,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG51" t="n">
+      <c r="AG51" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH51" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6745,7 +7000,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG52" t="n">
+      <c r="AG52" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH52" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6868,7 +7128,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG53" t="n">
+      <c r="AG53" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH53" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6995,7 +7260,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG54" t="n">
+      <c r="AG54" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH54" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7118,7 +7388,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG55" t="n">
+      <c r="AG55" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH55" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7237,7 +7512,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG56" t="n">
+      <c r="AG56" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH56" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7356,7 +7636,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG57" t="n">
+      <c r="AG57" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH57" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7475,7 +7760,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG58" t="n">
+      <c r="AG58" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH58" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7598,7 +7888,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG59" t="n">
+      <c r="AG59" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH59" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7717,7 +8012,12 @@
           <t>outside</t>
         </is>
       </c>
-      <c r="AG60" t="n">
+      <c r="AG60" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH60" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7836,7 +8136,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG61" t="n">
+      <c r="AG61" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH61" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7959,7 +8264,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG62" t="n">
+      <c r="AG62" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH62" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8082,7 +8392,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG63" t="n">
+      <c r="AG63" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH63" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8209,7 +8524,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG64" t="n">
+      <c r="AG64" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH64" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8332,7 +8652,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG65" t="n">
+      <c r="AG65" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH65" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8455,7 +8780,12 @@
           <t>outside</t>
         </is>
       </c>
-      <c r="AG66" t="n">
+      <c r="AG66" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH66" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8578,7 +8908,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG67" t="n">
+      <c r="AG67" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH67" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8701,7 +9036,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG68" t="n">
+      <c r="AG68" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH68" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8824,7 +9164,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG69" t="n">
+      <c r="AG69" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH69" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8943,7 +9288,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG70" t="n">
+      <c r="AG70" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH70" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9062,7 +9412,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG71" t="n">
+      <c r="AG71" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH71" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9185,7 +9540,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG72" t="n">
+      <c r="AG72" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH72" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9308,7 +9668,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG73" t="n">
+      <c r="AG73" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH73" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9427,7 +9792,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG74" t="n">
+      <c r="AG74" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH74" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9554,7 +9924,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG75" t="n">
+      <c r="AG75" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH75" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9677,7 +10052,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG76" t="n">
+      <c r="AG76" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH76" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9800,7 +10180,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG77" t="n">
+      <c r="AG77" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH77" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9923,7 +10308,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG78" t="n">
+      <c r="AG78" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH78" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10046,7 +10436,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG79" t="n">
+      <c r="AG79" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH79" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10165,7 +10560,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG80" t="n">
+      <c r="AG80" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH80" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10288,7 +10688,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG81" t="n">
+      <c r="AG81" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH81" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10411,7 +10816,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG82" t="n">
+      <c r="AG82" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH82" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10530,7 +10940,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG83" t="n">
+      <c r="AG83" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH83" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10649,7 +11064,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG84" t="n">
+      <c r="AG84" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH84" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10768,7 +11188,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG85" t="n">
+      <c r="AG85" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH85" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10891,7 +11316,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG86" t="n">
+      <c r="AG86" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH86" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11014,7 +11444,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG87" t="n">
+      <c r="AG87" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH87" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11133,7 +11568,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG88" t="n">
+      <c r="AG88" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH88" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11252,7 +11692,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG89" t="n">
+      <c r="AG89" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH89" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11375,7 +11820,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG90" t="n">
+      <c r="AG90" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH90" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11502,7 +11952,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG91" t="n">
+      <c r="AG91" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH91" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11625,7 +12080,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG92" t="n">
+      <c r="AG92" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH92" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11744,7 +12204,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG93" t="n">
+      <c r="AG93" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH93" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11863,7 +12328,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG94" t="n">
+      <c r="AG94" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH94" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11982,7 +12452,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG95" t="n">
+      <c r="AG95" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH95" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12101,7 +12576,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG96" t="n">
+      <c r="AG96" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH96" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12228,7 +12708,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG97" t="n">
+      <c r="AG97" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH97" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12351,7 +12836,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG98" t="n">
+      <c r="AG98" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH98" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12474,7 +12964,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG99" t="n">
+      <c r="AG99" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH99" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12593,7 +13088,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG100" t="n">
+      <c r="AG100" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH100" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12716,7 +13216,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG101" t="n">
+      <c r="AG101" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH101" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12839,7 +13344,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG102" t="n">
+      <c r="AG102" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH102" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12966,7 +13476,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG103" t="n">
+      <c r="AG103" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH103" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13089,7 +13604,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG104" t="n">
+      <c r="AG104" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH104" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13212,7 +13732,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG105" t="n">
+      <c r="AG105" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH105" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13335,7 +13860,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG106" t="n">
+      <c r="AG106" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH106" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13458,7 +13988,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG107" t="n">
+      <c r="AG107" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH107" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13581,7 +14116,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG108" t="n">
+      <c r="AG108" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH108" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13704,7 +14244,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG109" t="n">
+      <c r="AG109" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH109" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13831,7 +14376,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG110" t="n">
+      <c r="AG110" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH110" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13950,7 +14500,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG111" t="n">
+      <c r="AG111" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH111" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14069,7 +14624,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG112" t="n">
+      <c r="AG112" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH112" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14196,7 +14756,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG113" t="n">
+      <c r="AG113" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH113" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14323,7 +14888,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG114" t="n">
+      <c r="AG114" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH114" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14438,7 +15008,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG115" t="n">
+      <c r="AG115" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH115" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14557,7 +15132,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG116" t="n">
+      <c r="AG116" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH116" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14684,7 +15264,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG117" t="n">
+      <c r="AG117" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH117" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14803,7 +15388,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG118" t="n">
+      <c r="AG118" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH118" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14918,7 +15508,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG119" t="n">
+      <c r="AG119" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH119" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15037,7 +15632,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG120" t="n">
+      <c r="AG120" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH120" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15160,7 +15760,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG121" t="n">
+      <c r="AG121" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH121" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15287,7 +15892,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG122" t="n">
+      <c r="AG122" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH122" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15414,7 +16024,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG123" t="n">
+      <c r="AG123" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH123" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15529,7 +16144,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG124" t="n">
+      <c r="AG124" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH124" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15648,7 +16268,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG125" t="n">
+      <c r="AG125" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH125" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15771,7 +16396,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG126" t="n">
+      <c r="AG126" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH126" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15898,7 +16528,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG127" t="n">
+      <c r="AG127" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH127" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16017,7 +16652,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG128" t="n">
+      <c r="AG128" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH128" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16140,7 +16780,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG129" t="n">
+      <c r="AG129" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH129" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16263,7 +16908,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG130" t="n">
+      <c r="AG130" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH130" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16386,7 +17036,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG131" t="n">
+      <c r="AG131" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH131" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16509,7 +17164,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG132" t="n">
+      <c r="AG132" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH132" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16628,7 +17288,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG133" t="n">
+      <c r="AG133" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH133" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16755,7 +17420,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG134" t="n">
+      <c r="AG134" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH134" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16878,7 +17548,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG135" t="n">
+      <c r="AG135" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH135" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17001,7 +17676,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG136" t="n">
+      <c r="AG136" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH136" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17124,7 +17804,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG137" t="n">
+      <c r="AG137" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH137" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17243,7 +17928,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG138" t="n">
+      <c r="AG138" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH138" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17366,7 +18056,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG139" t="n">
+      <c r="AG139" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH139" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17485,7 +18180,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG140" t="n">
+      <c r="AG140" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH140" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17612,7 +18312,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG141" t="n">
+      <c r="AG141" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH141" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17731,7 +18436,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG142" t="n">
+      <c r="AG142" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH142" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17858,7 +18568,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG143" t="n">
+      <c r="AG143" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH143" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17981,7 +18696,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG144" t="n">
+      <c r="AG144" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH144" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18100,7 +18820,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG145" t="n">
+      <c r="AG145" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH145" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18227,7 +18952,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG146" t="n">
+      <c r="AG146" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH146" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18346,7 +19076,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG147" t="n">
+      <c r="AG147" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH147" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18469,7 +19204,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG148" t="n">
+      <c r="AG148" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH148" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18588,7 +19328,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG149" t="n">
+      <c r="AG149" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH149" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18707,7 +19452,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG150" t="n">
+      <c r="AG150" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH150" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18830,7 +19580,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG151" t="n">
+      <c r="AG151" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH151" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18945,7 +19700,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG152" t="n">
+      <c r="AG152" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH152" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19068,7 +19828,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG153" t="n">
+      <c r="AG153" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH153" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19187,7 +19952,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG154" t="n">
+      <c r="AG154" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH154" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19310,7 +20080,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG155" t="n">
+      <c r="AG155" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH155" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19429,7 +20204,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG156" t="n">
+      <c r="AG156" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH156" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19548,7 +20328,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG157" t="n">
+      <c r="AG157" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH157" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19671,7 +20456,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG158" t="n">
+      <c r="AG158" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH158" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19794,7 +20584,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG159" t="n">
+      <c r="AG159" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH159" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19917,7 +20712,12 @@
           <t>outside</t>
         </is>
       </c>
-      <c r="AG160" t="n">
+      <c r="AG160" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH160" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20040,7 +20840,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG161" t="n">
+      <c r="AG161" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH161" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20163,7 +20968,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG162" t="n">
+      <c r="AG162" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH162" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20282,7 +21092,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG163" t="n">
+      <c r="AG163" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH163" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20401,7 +21216,12 @@
           <t>outside</t>
         </is>
       </c>
-      <c r="AG164" t="n">
+      <c r="AG164" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH164" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20524,7 +21344,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG165" t="n">
+      <c r="AG165" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH165" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20643,7 +21468,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG166" t="n">
+      <c r="AG166" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH166" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20766,7 +21596,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG167" t="n">
+      <c r="AG167" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH167" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20881,7 +21716,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG168" t="n">
+      <c r="AG168" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH168" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21004,7 +21844,12 @@
           <t>outside</t>
         </is>
       </c>
-      <c r="AG169" t="n">
+      <c r="AG169" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH169" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21123,7 +21968,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG170" t="n">
+      <c r="AG170" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH170" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21242,7 +22092,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG171" t="n">
+      <c r="AG171" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH171" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21365,7 +22220,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG172" t="n">
+      <c r="AG172" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH172" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21488,7 +22348,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG173" t="n">
+      <c r="AG173" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH173" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21611,7 +22476,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG174" t="n">
+      <c r="AG174" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH174" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21730,7 +22600,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG175" t="n">
+      <c r="AG175" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH175" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21845,7 +22720,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG176" t="n">
+      <c r="AG176" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH176" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21964,7 +22844,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG177" t="n">
+      <c r="AG177" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH177" t="n">
         <v>5</v>
       </c>
     </row>
@@ -22087,7 +22972,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG178" t="n">
+      <c r="AG178" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH178" t="n">
         <v>5</v>
       </c>
     </row>
@@ -22210,7 +23100,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG179" t="n">
+      <c r="AG179" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="AH179" t="n">
         <v>5</v>
       </c>
     </row>
@@ -22329,7 +23224,12 @@
           <t>inside</t>
         </is>
       </c>
-      <c r="AG180" t="n">
+      <c r="AG180" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="AH180" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>